<commit_message>
Updated Acetone Folder with corrected Temperatures
</commit_message>
<xml_diff>
--- a/Acetone/Acetone_AVE_MASS_FRAC.xlsx
+++ b/Acetone/Acetone_AVE_MASS_FRAC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Git_Repos\Pool_Fires\Acetone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{12E90D77-F153-41E5-8322-75FCEE7B0BFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{EBDD96B5-3063-4162-A7AB-14DA5457C350}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="11055" xr2:uid="{BCA13EF2-66E1-465B-9C70-A0EB7B3DF54C}"/>
+    <workbookView xWindow="25200" yWindow="-11550" windowWidth="16200" windowHeight="10980" xr2:uid="{BCA13EF2-66E1-465B-9C70-A0EB7B3DF54C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE688D5-8342-4704-9FD2-F973946AFFE0}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,19 +610,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6.3324815531486459E-2</v>
+        <v>6.8638420465574931E-2</v>
       </c>
       <c r="C2">
-        <v>7.2647552018043646E-4</v>
+        <v>7.9908414990062212E-4</v>
       </c>
       <c r="D2">
-        <v>2.7068070663292258E-2</v>
+        <v>3.4309510481396133E-2</v>
       </c>
       <c r="E2">
-        <v>2.7632059127537007E-3</v>
+        <v>3.0834031642105702E-3</v>
       </c>
       <c r="F2">
-        <v>2.0421270237036012E-4</v>
+        <v>3.2962744917057626E-4</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -631,34 +631,34 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.18199640372573356</v>
+        <v>0.19327013256176639</v>
       </c>
       <c r="J2">
-        <v>8.1207366898582725E-2</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1.0030115814189012E-2</v>
+        <v>1.1279529457069951E-2</v>
       </c>
       <c r="L2">
-        <v>0.56557173128622107</v>
+        <v>0.63424208791346104</v>
       </c>
       <c r="M2">
-        <v>4.0600576106341178E-2</v>
+        <v>3.6419103276155038E-2</v>
       </c>
       <c r="N2">
-        <v>1.8034440852684391E-2</v>
+        <v>1.1914908462461746E-2</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>1.3223940334868239E-3</v>
+        <v>9.3754918274818473E-4</v>
       </c>
       <c r="Q2">
-        <v>2.9455279005555948E-3</v>
+        <v>1.8747004808270912E-3</v>
       </c>
       <c r="R2">
-        <v>4.2046630521223871E-3</v>
+        <v>2.9019429552577971E-3</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -666,19 +666,19 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>8.1267679461571291E-2</v>
+        <v>8.3951639954735424E-2</v>
       </c>
       <c r="C3">
-        <v>1.0242015472722735E-3</v>
+        <v>9.9763912451076089E-4</v>
       </c>
       <c r="D3">
-        <v>2.9813129926940445E-2</v>
+        <v>3.8590242365482308E-2</v>
       </c>
       <c r="E3">
-        <v>3.6804997794353655E-3</v>
+        <v>3.8475542626794017E-3</v>
       </c>
       <c r="F3">
-        <v>1.5889639203151587E-4</v>
+        <v>8.7760468436844409E-5</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -687,34 +687,34 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.24142187950506669</v>
+        <v>0.24229601012811072</v>
       </c>
       <c r="J3">
-        <v>1.7032130123162455E-2</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>1.3819869661150199E-2</v>
+        <v>1.4395326538266374E-2</v>
       </c>
       <c r="L3">
-        <v>0.52287060575620592</v>
+        <v>0.54694655225996702</v>
       </c>
       <c r="M3">
-        <v>5.4483666127500122E-2</v>
+        <v>4.6707508031712988E-2</v>
       </c>
       <c r="N3">
-        <v>2.2445885422010668E-2</v>
+        <v>1.4503468454741117E-2</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>2.264281954946649E-3</v>
+        <v>1.4136335505368191E-3</v>
       </c>
       <c r="Q3">
-        <v>3.9896939749912734E-3</v>
+        <v>2.4361528429249031E-3</v>
       </c>
       <c r="R3">
-        <v>5.727580367715303E-3</v>
+        <v>3.8265120178952805E-3</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -722,19 +722,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.1020242186648169</v>
+        <v>0.10693683020356214</v>
       </c>
       <c r="C4">
-        <v>1.2517248410757612E-3</v>
+        <v>1.2956404020672083E-3</v>
       </c>
       <c r="D4">
-        <v>3.4811242707898489E-2</v>
+        <v>4.3728301883223838E-2</v>
       </c>
       <c r="E4">
-        <v>4.9224905353001738E-3</v>
+        <v>5.2656210920229134E-3</v>
       </c>
       <c r="F4">
-        <v>3.5133726673587255E-4</v>
+        <v>2.4463660168600452E-4</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -743,34 +743,34 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.31661846630968482</v>
+        <v>0.32347423487878285</v>
       </c>
       <c r="J4">
-        <v>1.816710037491891E-2</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1.7774355786933597E-2</v>
+        <v>1.9013050847986712E-2</v>
       </c>
       <c r="L4">
-        <v>0.39139003560356406</v>
+        <v>0.41364821603005553</v>
       </c>
       <c r="M4">
-        <v>6.9497088883965469E-2</v>
+        <v>5.8311481814932696E-2</v>
       </c>
       <c r="N4">
-        <v>2.8389977045371193E-2</v>
+        <v>1.8546154195211547E-2</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>3.0012975271481199E-3</v>
+        <v>1.9482838823551576E-3</v>
       </c>
       <c r="Q4">
-        <v>4.4686984561895966E-3</v>
+        <v>2.8053491118048518E-3</v>
       </c>
       <c r="R4">
-        <v>7.3319659963972262E-3</v>
+        <v>4.7821990563085472E-3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -778,19 +778,19 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.12745982224051652</v>
+        <v>0.1283185967356951</v>
       </c>
       <c r="C5">
-        <v>1.5565158196447625E-3</v>
+        <v>1.5081516002418826E-3</v>
       </c>
       <c r="D5">
-        <v>4.4404039180830211E-2</v>
+        <v>5.9489121816044134E-2</v>
       </c>
       <c r="E5">
-        <v>6.7386975538738427E-3</v>
+        <v>6.9522600485077655E-3</v>
       </c>
       <c r="F5">
-        <v>2.0541608021355262E-3</v>
+        <v>1.9355192791594713E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -799,34 +799,34 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.43614530329112616</v>
+        <v>0.42328813296804463</v>
       </c>
       <c r="J5">
-        <v>1.3910954782385292E-2</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>2.2356185600133409E-2</v>
+        <v>2.218886819733951E-2</v>
       </c>
       <c r="L5">
-        <v>0.2060740876930367</v>
+        <v>0.25269436522415017</v>
       </c>
       <c r="M5">
-        <v>8.9988012749325899E-2</v>
+        <v>7.2112054708959455E-2</v>
       </c>
       <c r="N5">
-        <v>3.1469986727312604E-2</v>
+        <v>1.9979329412226379E-2</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>3.8564783196957711E-3</v>
+        <v>2.49042543049279E-3</v>
       </c>
       <c r="Q5">
-        <v>5.1364172934344676E-3</v>
+        <v>3.2052431773109567E-3</v>
       </c>
       <c r="R5">
-        <v>8.8493379465488277E-3</v>
+        <v>5.8379314018277562E-3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -834,19 +834,19 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>0.13426263527141816</v>
+        <v>0.13634068049614936</v>
       </c>
       <c r="C6">
-        <v>1.5676101780619123E-3</v>
+        <v>1.632433023356703E-3</v>
       </c>
       <c r="D6">
-        <v>4.8575793022857153E-2</v>
+        <v>6.7359121538423952E-2</v>
       </c>
       <c r="E6">
-        <v>8.7066413087136044E-3</v>
+        <v>9.0678002511428157E-3</v>
       </c>
       <c r="F6">
-        <v>1.4305828298975396E-2</v>
+        <v>1.3941672521544143E-2</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -855,34 +855,34 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.54364495777333288</v>
+        <v>0.54247199218170927</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>1.9339548543349846E-2</v>
+        <v>2.0125956592672013E-2</v>
       </c>
       <c r="L6">
-        <v>0.10897959207235147</v>
+        <v>0.11293835281919416</v>
       </c>
       <c r="M6">
-        <v>8.2920684629817124E-2</v>
+        <v>7.2436385240713608E-2</v>
       </c>
       <c r="N6">
-        <v>2.3049985538359647E-2</v>
+        <v>1.4438892038429688E-2</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>3.1181759561891122E-3</v>
+        <v>1.8737120062576134E-3</v>
       </c>
       <c r="Q6">
-        <v>4.1452333453972966E-3</v>
+        <v>2.4933500182573254E-3</v>
       </c>
       <c r="R6">
-        <v>7.3833140611763645E-3</v>
+        <v>4.8796512721491977E-3</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -890,19 +890,19 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>0.12944567426908629</v>
+        <v>0.13021727854361778</v>
       </c>
       <c r="C7">
-        <v>1.297312800249446E-3</v>
+        <v>1.3562041710173218E-3</v>
       </c>
       <c r="D7">
-        <v>4.6234078424782561E-2</v>
+        <v>6.1024042497776099E-2</v>
       </c>
       <c r="E7">
-        <v>9.2687185594564712E-3</v>
+        <v>1.0282461397742729E-2</v>
       </c>
       <c r="F7">
-        <v>2.689584808478087E-2</v>
+        <v>2.7335712178824141E-2</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -911,34 +911,34 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.5993625772891894</v>
+        <v>0.60353350827993602</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>1.7360177333380043E-2</v>
+        <v>1.7998475069833833E-2</v>
       </c>
       <c r="L7">
-        <v>6.3606920651724325E-2</v>
+        <v>6.6477315898014547E-2</v>
       </c>
       <c r="M7">
-        <v>7.6174352074803039E-2</v>
+        <v>6.2540286985648341E-2</v>
       </c>
       <c r="N7">
-        <v>1.7373135082282762E-2</v>
+        <v>1.0824665781917582E-2</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>2.7701713640581973E-3</v>
+        <v>1.6455035889346744E-3</v>
       </c>
       <c r="Q7">
-        <v>3.5456786907266482E-3</v>
+        <v>2.3048291886861609E-3</v>
       </c>
       <c r="R7">
-        <v>6.6653553754799349E-3</v>
+        <v>4.4597164180508212E-3</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -946,19 +946,19 @@
         <v>30</v>
       </c>
       <c r="B8">
-        <v>9.353853467926726E-2</v>
+        <v>9.5515391681124787E-2</v>
       </c>
       <c r="C8">
-        <v>7.4157495961934845E-4</v>
+        <v>8.0658242890213866E-4</v>
       </c>
       <c r="D8">
-        <v>3.9394150367718796E-2</v>
+        <v>4.9336862137483894E-2</v>
       </c>
       <c r="E8">
-        <v>1.0746860959416694E-2</v>
+        <v>1.1035600912545213E-2</v>
       </c>
       <c r="F8">
-        <v>7.9295850654788572E-2</v>
+        <v>7.9987025985359672E-2</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -967,34 +967,34 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0.69607516349854959</v>
+        <v>0.69125397887916096</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>8.5401633350638793E-3</v>
+        <v>8.6748261110099305E-3</v>
       </c>
       <c r="L8">
-        <v>1.4953169019467791E-2</v>
+        <v>1.5372523488123645E-2</v>
       </c>
       <c r="M8">
-        <v>4.3034726922551406E-2</v>
+        <v>4.0859639845888689E-2</v>
       </c>
       <c r="N8">
-        <v>7.9633460073855657E-3</v>
+        <v>3.5325665617994963E-3</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>1.0213953653298213E-3</v>
+        <v>6.2654634271975076E-4</v>
       </c>
       <c r="Q8">
-        <v>1.472116709441716E-3</v>
+        <v>8.8309907458642225E-4</v>
       </c>
       <c r="R8">
-        <v>3.2229475213994764E-3</v>
+        <v>2.1153565512951854E-3</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1002,19 +1002,19 @@
         <v>45</v>
       </c>
       <c r="B9">
-        <v>7.1921404912506454E-2</v>
+        <v>7.179667711319962E-2</v>
       </c>
       <c r="C9">
-        <v>2.1553722312249142E-4</v>
+        <v>2.1289565555455319E-4</v>
       </c>
       <c r="D9">
-        <v>2.3105764989475228E-2</v>
+        <v>4.2039180019614694E-2</v>
       </c>
       <c r="E9">
-        <v>1.1503745716832254E-2</v>
+        <v>1.1594908268795131E-2</v>
       </c>
       <c r="F9">
-        <v>0.11863392733369567</v>
+        <v>0.11818525920305735</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1023,34 +1023,34 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.74742433363641092</v>
+        <v>0.72687452684243659</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>2.970093607517676E-3</v>
+        <v>2.9552362372269663E-3</v>
       </c>
       <c r="L9">
-        <v>1.8770844484923617E-3</v>
+        <v>1.8900747527759931E-3</v>
       </c>
       <c r="M9">
-        <v>1.7924251172603906E-2</v>
+        <v>2.2032642373279888E-2</v>
       </c>
       <c r="N9">
-        <v>2.6510574565238765E-3</v>
+        <v>1.3149801784385264E-3</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
-        <v>3.6702937770853708E-4</v>
+        <v>2.20525098798073E-4</v>
       </c>
       <c r="Q9">
-        <v>3.743632267995267E-4</v>
+        <v>2.1998597260094153E-4</v>
       </c>
       <c r="R9">
-        <v>1.0314068983111328E-3</v>
+        <v>6.6310828422173809E-4</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1058,19 +1058,19 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <v>4.1508721664377905E-2</v>
+        <v>5.3270244601418326E-2</v>
       </c>
       <c r="C10">
-        <v>6.1767965033083833E-5</v>
+        <v>1.2379244280364573E-4</v>
       </c>
       <c r="D10">
-        <v>1.1559011304194542E-2</v>
+        <v>2.4259918294598743E-2</v>
       </c>
       <c r="E10">
-        <v>1.1783769257067377E-2</v>
+        <v>1.1944736397900512E-2</v>
       </c>
       <c r="F10">
-        <v>0.17099874507071203</v>
+        <v>0.15849046663082639</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1079,22 +1079,22 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.76027875951049628</v>
+        <v>0.74313595078462813</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>3.8741390164427327E-4</v>
+        <v>6.7007407352815416E-4</v>
       </c>
       <c r="L10">
-        <v>9.630252362850682E-5</v>
+        <v>1.2299327245527121E-4</v>
       </c>
       <c r="M10">
-        <v>3.030573257782825E-3</v>
+        <v>7.4919671116218441E-3</v>
       </c>
       <c r="N10">
-        <v>1.7920791218147108E-4</v>
+        <v>3.6542313511610339E-4</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1103,65 +1103,121 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>1.8699242529182946E-5</v>
+        <v>2.2287971743192615E-5</v>
       </c>
       <c r="R10">
-        <v>9.7028390352569191E-5</v>
+        <v>1.0214528335972133E-4</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>3.6681189601409606E-2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1.6684162082519993E-2</v>
+      </c>
+      <c r="E11">
+        <v>1.2141612930736128E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.183389754119925</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.74979246824134915</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>6.8216024083202133E-5</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1.2425969999767966E-3</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>100</v>
       </c>
-      <c r="B11">
-        <v>2.2881222811295017E-2</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>3.8363604352541101E-3</v>
-      </c>
-      <c r="E11">
-        <v>1.1835185767070901E-2</v>
-      </c>
-      <c r="F11">
-        <v>0.19752619303463628</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0.76359275308986174</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>1.0843779035774792E-4</v>
-      </c>
-      <c r="M11">
-        <v>2.1984707152410084E-4</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
+      <c r="B12">
+        <v>1.8068094369527492E-2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>7.6393135862394207E-3</v>
+      </c>
+      <c r="E12">
+        <v>1.2196932867977741E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.20295961794891021</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.75896386932232407</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1.1987868108138962E-5</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1.6018403691292216E-4</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
         <v>0</v>
       </c>
     </row>
@@ -1172,7 +1228,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF55484-0DC5-47A1-8E1B-E2AED1735F61}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1258,19 +1314,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5.553635973196803E-3</v>
+        <v>5.2146980384027465E-3</v>
       </c>
       <c r="C2">
-        <v>6.825161839899108E-5</v>
+        <v>8.6317707290217341E-5</v>
       </c>
       <c r="D2">
-        <v>5.6250394408425925E-3</v>
+        <v>7.0731780948885686E-3</v>
       </c>
       <c r="E2">
-        <v>2.5053832358014165E-4</v>
+        <v>3.4586985105102024E-4</v>
       </c>
       <c r="F2">
-        <v>1.7763734428754699E-5</v>
+        <v>4.2941893721008231E-4</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1279,34 +1335,34 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1.5888618572078506E-2</v>
+        <v>1.568358785728334E-2</v>
       </c>
       <c r="J2">
-        <v>0.13790734094091686</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>9.972725181807173E-4</v>
+        <v>1.3177097479420098E-3</v>
       </c>
       <c r="L2">
-        <v>6.341678035845201E-2</v>
+        <v>7.7484762571971275E-2</v>
       </c>
       <c r="M2">
-        <v>3.5555959621863279E-3</v>
+        <v>9.3230745584893405E-3</v>
       </c>
       <c r="N2">
-        <v>4.5401613113744107E-3</v>
+        <v>3.0144287268773231E-3</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>6.1862532662647894E-4</v>
+        <v>2.1715221609071216E-4</v>
       </c>
       <c r="Q2">
-        <v>2.8041001051690037E-4</v>
+        <v>2.356182119527143E-4</v>
       </c>
       <c r="R2">
-        <v>4.1356944151420359E-4</v>
+        <v>2.7276841935601048E-4</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1314,19 +1370,19 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>4.3014615831999566E-3</v>
+        <v>4.627390166709996E-3</v>
       </c>
       <c r="C3">
-        <v>6.3245859577180249E-5</v>
+        <v>1.1983615993016051E-4</v>
       </c>
       <c r="D3">
-        <v>1.2815910702197312E-2</v>
+        <v>8.8743403945173178E-3</v>
       </c>
       <c r="E3">
-        <v>2.0570910061792788E-4</v>
+        <v>3.6019075733782551E-4</v>
       </c>
       <c r="F3">
-        <v>5.482687970123912E-5</v>
+        <v>3.3118931432930436E-5</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1335,34 +1391,34 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1.2595021453962928E-2</v>
+        <v>1.2435200387784342E-2</v>
       </c>
       <c r="J3">
-        <v>2.7951662142775519E-2</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>9.6123214011261217E-4</v>
+        <v>1.0305937178930252E-3</v>
       </c>
       <c r="L3">
-        <v>4.960387849882221E-2</v>
+        <v>5.2220114333225258E-2</v>
       </c>
       <c r="M3">
-        <v>2.7995271846603148E-3</v>
+        <v>1.0024045354051879E-2</v>
       </c>
       <c r="N3">
-        <v>5.3861633463495786E-3</v>
+        <v>3.4626964531113392E-3</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>1.0823491289345853E-3</v>
+        <v>3.3348985268507133E-4</v>
       </c>
       <c r="Q3">
-        <v>2.5129090023473012E-4</v>
+        <v>1.5653114338290557E-4</v>
       </c>
       <c r="R3">
-        <v>4.2209380937003894E-4</v>
+        <v>2.9456080989021178E-4</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1370,19 +1426,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7.236027328107456E-3</v>
+        <v>1.3325983773995754E-2</v>
       </c>
       <c r="C4">
-        <v>8.6928819306982411E-5</v>
+        <v>1.6583596212898344E-4</v>
       </c>
       <c r="D4">
-        <v>7.3159263374412342E-3</v>
+        <v>1.054232993935655E-2</v>
       </c>
       <c r="E4">
-        <v>5.9487091636943503E-4</v>
+        <v>8.9586781916399462E-4</v>
       </c>
       <c r="F4">
-        <v>3.7939703643236571E-4</v>
+        <v>3.8806837910591689E-4</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1391,34 +1447,34 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>3.8744537588191602E-2</v>
+        <v>4.8016824983081192E-2</v>
       </c>
       <c r="J4">
-        <v>3.2570543523486192E-2</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1.6630364695945318E-3</v>
+        <v>2.6527026514707266E-3</v>
       </c>
       <c r="L4">
-        <v>0.13114844629575084</v>
+        <v>0.14947363489614621</v>
       </c>
       <c r="M4">
-        <v>4.5113920241558747E-3</v>
+        <v>8.3462374159450851E-3</v>
       </c>
       <c r="N4">
-        <v>3.1782817083732895E-3</v>
+        <v>2.9191583282103251E-3</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>1.3918416424105633E-3</v>
+        <v>4.6736991630810744E-4</v>
       </c>
       <c r="Q4">
-        <v>3.8219024809744257E-4</v>
+        <v>4.2025348462503264E-4</v>
       </c>
       <c r="R4">
-        <v>5.7204911499591268E-4</v>
+        <v>6.2315916418519655E-4</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1426,19 +1482,19 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>5.6214102178233204E-3</v>
+        <v>9.5248925047054268E-3</v>
       </c>
       <c r="C5">
-        <v>8.6384359639858006E-5</v>
+        <v>2.1028437084416729E-4</v>
       </c>
       <c r="D5">
-        <v>8.5918133875261971E-3</v>
+        <v>1.2036061428864507E-2</v>
       </c>
       <c r="E5">
-        <v>3.3522078956421116E-4</v>
+        <v>6.9748007318369001E-4</v>
       </c>
       <c r="F5">
-        <v>8.7641219746434221E-5</v>
+        <v>1.6361981513756763E-4</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1447,34 +1503,34 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1.8887108455882054E-2</v>
+        <v>3.5224873550377067E-2</v>
       </c>
       <c r="J5">
-        <v>3.5180870123147683E-2</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1.438385971037084E-3</v>
+        <v>1.9539468368948714E-3</v>
       </c>
       <c r="L5">
-        <v>1.7026396735868914E-2</v>
+        <v>8.7140422532264866E-2</v>
       </c>
       <c r="M5">
-        <v>3.9462224439355707E-3</v>
+        <v>5.4375623690310218E-3</v>
       </c>
       <c r="N5">
-        <v>1.7334296008477161E-3</v>
+        <v>1.5293555969379655E-3</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>1.780244840466777E-3</v>
+        <v>5.2676376421930662E-4</v>
       </c>
       <c r="Q5">
-        <v>2.9579908874722129E-4</v>
+        <v>2.6610259548824524E-4</v>
       </c>
       <c r="R5">
-        <v>5.5464344746626137E-4</v>
+        <v>6.0107322726180804E-4</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1482,19 +1538,19 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>7.1701969477627626E-3</v>
+        <v>7.4310775376446175E-3</v>
       </c>
       <c r="C6">
-        <v>6.6398808994748101E-5</v>
+        <v>1.2122991374817747E-4</v>
       </c>
       <c r="D6">
-        <v>1.3675332384556781E-2</v>
+        <v>2.2833267121986561E-2</v>
       </c>
       <c r="E6">
-        <v>4.9872490456192274E-4</v>
+        <v>1.0751258427360326E-3</v>
       </c>
       <c r="F6">
-        <v>1.3452466554809315E-2</v>
+        <v>1.3090046750940464E-2</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1503,34 +1559,34 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>3.8136202259608773E-2</v>
+        <v>4.906524998422683E-2</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>3.1033538386884417E-3</v>
+        <v>2.4995707432602411E-3</v>
       </c>
       <c r="L6">
-        <v>2.0227175161866208E-2</v>
+        <v>2.028474479401484E-2</v>
       </c>
       <c r="M6">
-        <v>8.4022672685109892E-3</v>
+        <v>8.4753491081191734E-3</v>
       </c>
       <c r="N6">
-        <v>5.4446349819349529E-3</v>
+        <v>3.5870124288600474E-3</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>1.5910214467298471E-3</v>
+        <v>4.0373460525062164E-4</v>
       </c>
       <c r="Q6">
-        <v>3.2223086187719457E-4</v>
+        <v>3.0136234148151961E-4</v>
       </c>
       <c r="R6">
-        <v>9.8991205940940114E-4</v>
+        <v>6.4016565778674548E-4</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1538,19 +1594,19 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>1.0977372168292535E-2</v>
+        <v>1.1031979069653749E-2</v>
       </c>
       <c r="C7">
-        <v>2.0989217080968523E-4</v>
+        <v>2.1151330261691347E-4</v>
       </c>
       <c r="D7">
-        <v>1.1453109218462536E-2</v>
+        <v>1.1885026850516525E-2</v>
       </c>
       <c r="E7">
-        <v>1.2452876846833203E-3</v>
+        <v>1.9987505585005562E-3</v>
       </c>
       <c r="F7">
-        <v>2.8880578904498952E-2</v>
+        <v>2.9657792840352849E-2</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1559,34 +1615,34 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>8.3454593477204492E-2</v>
+        <v>8.7638695886103346E-2</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>5.4548840221346345E-3</v>
+        <v>5.4619635297072791E-3</v>
       </c>
       <c r="L7">
-        <v>2.9325257289217047E-2</v>
+        <v>3.0389678000023932E-2</v>
       </c>
       <c r="M7">
-        <v>1.8087399470322681E-2</v>
+        <v>2.2292421412055549E-2</v>
       </c>
       <c r="N7">
-        <v>1.02830202276681E-2</v>
+        <v>6.0553196179566129E-3</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>1.6526078819456991E-3</v>
+        <v>8.614458701125409E-4</v>
       </c>
       <c r="Q7">
-        <v>9.9510216468814321E-4</v>
+        <v>5.4534811768024822E-4</v>
       </c>
       <c r="R7">
-        <v>1.8727763633635841E-3</v>
+        <v>1.2102409831355563E-3</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1594,19 +1650,19 @@
         <v>30</v>
       </c>
       <c r="B8">
-        <v>2.2666440529201925E-2</v>
+        <v>2.2239542079306552E-2</v>
       </c>
       <c r="C8">
-        <v>2.2847999214165151E-4</v>
+        <v>3.2318456715713285E-4</v>
       </c>
       <c r="D8">
-        <v>1.2354657989158708E-2</v>
+        <v>1.7083920944618951E-2</v>
       </c>
       <c r="E8">
-        <v>8.463217478690831E-4</v>
+        <v>1.1530575181502485E-3</v>
       </c>
       <c r="F8">
-        <v>3.7885151431217269E-2</v>
+        <v>3.6953147451188002E-2</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1615,34 +1671,34 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>5.6585287775579675E-2</v>
+        <v>5.8650807457397126E-2</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>3.1503415299875513E-3</v>
+        <v>3.174997297723455E-3</v>
       </c>
       <c r="L8">
-        <v>3.3664103380314212E-3</v>
+        <v>3.4155685011927738E-3</v>
       </c>
       <c r="M8">
-        <v>1.3587763535549933E-2</v>
+        <v>2.457525135632295E-2</v>
       </c>
       <c r="N8">
-        <v>1.8665562540261886E-4</v>
+        <v>1.5794596747419384E-3</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>5.212930291521111E-4</v>
+        <v>1.8288720041739672E-4</v>
       </c>
       <c r="Q8">
-        <v>4.5677629017961758E-4</v>
+        <v>2.714482848128302E-4</v>
       </c>
       <c r="R8">
-        <v>1.0806747454003482E-3</v>
+        <v>7.0452201746111617E-4</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1650,19 +1706,19 @@
         <v>45</v>
       </c>
       <c r="B9">
-        <v>1.0016593832282837E-2</v>
+        <v>9.958801289692943E-3</v>
       </c>
       <c r="C9">
-        <v>3.1217862239878462E-4</v>
+        <v>3.0832511964708453E-4</v>
       </c>
       <c r="D9">
-        <v>1.3132430217861093E-2</v>
+        <v>8.754045328446947E-3</v>
       </c>
       <c r="E9">
-        <v>3.9766695829573435E-4</v>
+        <v>8.3735440454441826E-4</v>
       </c>
       <c r="F9">
-        <v>8.8886326391467291E-3</v>
+        <v>7.9733286958483737E-3</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1671,34 +1727,34 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1.8203396056856568E-2</v>
+        <v>1.8337123462245211E-2</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>1.0865101381563411E-3</v>
+        <v>1.0787683690666662E-3</v>
       </c>
       <c r="L9">
-        <v>5.3003342200129281E-4</v>
+        <v>5.3191164601807891E-4</v>
       </c>
       <c r="M9">
-        <v>5.4844400102217359E-3</v>
+        <v>6.9570745458305289E-3</v>
       </c>
       <c r="N9">
-        <v>5.7359901901820221E-4</v>
+        <v>1.6034720724248695E-4</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
-        <v>1.7717394549243291E-4</v>
+        <v>5.3977750699421105E-5</v>
       </c>
       <c r="Q9">
-        <v>4.1017185154718669E-5</v>
+        <v>2.3998589204111956E-5</v>
       </c>
       <c r="R9">
-        <v>2.9527312722410915E-4</v>
+        <v>1.89817216907323E-4</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1706,19 +1762,19 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <v>2.055169388652045E-2</v>
+        <v>1.1863508312591781E-3</v>
       </c>
       <c r="C10">
-        <v>1.2358698157668313E-4</v>
+        <v>5.7953084413769532E-6</v>
       </c>
       <c r="D10">
-        <v>2.1987100905567678E-3</v>
+        <v>4.5965958666935288E-3</v>
       </c>
       <c r="E10">
-        <v>4.8893012204316371E-4</v>
+        <v>8.3916813936753189E-4</v>
       </c>
       <c r="F10">
-        <v>2.8819942706795547E-2</v>
+        <v>3.0541914864323817E-3</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1727,22 +1783,22 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2.8999052800261008E-2</v>
+        <v>1.4191096457776411E-2</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>4.9391349725538163E-4</v>
+        <v>3.4757039063320218E-5</v>
       </c>
       <c r="L10">
-        <v>4.8828670573055397E-5</v>
+        <v>8.9170323637937665E-6</v>
       </c>
       <c r="M10">
-        <v>3.6372462256238579E-3</v>
+        <v>1.6377960342791375E-4</v>
       </c>
       <c r="N10">
-        <v>3.3030921091296069E-6</v>
+        <v>4.4455303256145942E-6</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1751,65 +1807,121 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>3.7416148956397708E-5</v>
+        <v>9.5848990410756813E-7</v>
       </c>
       <c r="R10">
-        <v>1.1938311646256694E-4</v>
+        <v>5.4839387877996782E-6</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>8.1066321786174415E-4</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>3.1608632750471724E-3</v>
+      </c>
+      <c r="E11">
+        <v>8.5234680503798574E-4</v>
+      </c>
+      <c r="F11">
+        <v>3.4978991723778928E-3</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1.416919573520996E-2</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>3.533426693668802E-6</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>2.6948574960084141E-5</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>100</v>
       </c>
-      <c r="B11">
-        <v>5.2229093740313126E-4</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>7.2804950674693937E-4</v>
-      </c>
-      <c r="E11">
-        <v>3.8657781607415252E-4</v>
-      </c>
-      <c r="F11">
-        <v>4.1467671783749294E-3</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>1.6220119941363662E-2</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>7.9703144149078107E-6</v>
-      </c>
-      <c r="M11">
-        <v>4.9109616003819709E-6</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
+      <c r="B12">
+        <v>3.9786479109630527E-4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1.4472191713162117E-3</v>
+      </c>
+      <c r="E12">
+        <v>8.5592381012904878E-4</v>
+      </c>
+      <c r="F12">
+        <v>3.8523539927161447E-3</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1.4271504244954195E-2</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>6.2053455243985606E-7</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>3.4609083952881079E-6</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
         <v>0</v>
       </c>
     </row>

</xml_diff>